<commit_message>
Delete,Edit,List label and add use_model
</commit_message>
<xml_diff>
--- a/Text Annotation Tool Features.xlsx
+++ b/Text Annotation Tool Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Text-annotation-for-human\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CAC068-608E-458F-8356-17ACEA606BE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485BF2D1-EF73-43FB-A158-B8A1399C467F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>No.</t>
   </si>
@@ -594,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y907"/>
+  <dimension ref="A1:Y906"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -853,7 +853,9 @@
         <v>18</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="9"/>
+      <c r="F11" s="15" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -943,91 +945,88 @@
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>17</v>
-      </c>
-      <c r="B18" s="17"/>
+        <v>18</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="C18" s="6">
-        <v>3.5</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+        <v>27</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="15" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>18</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>26</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B19" s="18"/>
       <c r="C19" s="6">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E19" s="7"/>
-      <c r="F19" s="9"/>
+      <c r="F19" s="15" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>19</v>
-      </c>
-      <c r="B20" s="18"/>
+        <v>20</v>
+      </c>
+      <c r="B20" s="17"/>
       <c r="C20" s="6">
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E20" s="7"/>
-      <c r="F20" s="9"/>
+      <c r="F20" s="15" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>20</v>
-      </c>
-      <c r="B21" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="C21" s="6">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E21" s="12"/>
       <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>21</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>30</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B22" s="17"/>
       <c r="C22" s="6">
-        <v>5.0999999999999996</v>
+        <v>5.2</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="12"/>
+        <v>32</v>
+      </c>
+      <c r="E22" s="7"/>
       <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>22</v>
-      </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="6">
-        <v>5.2</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="9"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="14"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
@@ -5444,19 +5443,14 @@
       <c r="B906" s="13"/>
       <c r="C906" s="14"/>
     </row>
-    <row r="907" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A907" s="13"/>
-      <c r="B907" s="13"/>
-      <c r="C907" s="14"/>
-    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B9:B13"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B18:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>